<commit_message>
bj: update sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2024/Oct 2024/bj_sch_sth_impact_2410_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2024/Oct 2024/bj_sch_sth_impact_2410_2_child.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\Oct 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2024\Oct 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F010931-9C28-4A21-A122-9450B3EC3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E041D58F-0792-4436-A7E5-5AA3085B3B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="239">
   <si>
     <t>type</t>
   </si>
@@ -181,15 +181,6 @@
     <t>Was a stool sample successfully collected from this child?</t>
   </si>
   <si>
-    <t>*We do not want to come back to the house if they don’t give a sample as we can’t guarantee there won’t be any swapping of samples.</t>
-  </si>
-  <si>
-    <t>Un échantillon de selles de cet enfant a-t-il été prélevé ?</t>
-  </si>
-  <si>
-    <t>Nous ne voulons pas rentrer s'ils ne donnent pas d'échantillon car nous ne pouvons pas garantir qu'il n'y aura pas d'échange d'échantillons.</t>
-  </si>
-  <si>
     <t>Un échantillon d’urine de cet enfant a-t-il été prélevé ?</t>
   </si>
   <si>
@@ -211,21 +202,12 @@
     <t>The urine should not be conserved if the hemastix test result is positive</t>
   </si>
   <si>
-    <t>L'urine ne doit pas être conservée si le résultat du test Hemastix est positif</t>
-  </si>
-  <si>
     <t>You just entered a value that will end the survey</t>
   </si>
   <si>
     <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête</t>
   </si>
   <si>
-    <t>You have just entered a value that will cause the survey to end. Please collect the participant's stool and urine samples.</t>
-  </si>
-  <si>
-    <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête. Veuillez collecter les échantillons de selle et d'urine du participant.</t>
-  </si>
-  <si>
     <t>Additional notes</t>
   </si>
   <si>
@@ -709,9 +691,6 @@
     <t>p_espen_code_id</t>
   </si>
   <si>
-    <t>p_collected_stool</t>
-  </si>
-  <si>
     <t>p_collected_urine</t>
   </si>
   <si>
@@ -736,21 +715,12 @@
     <t>${p_consent} = 'A.donne'</t>
   </si>
   <si>
-    <t xml:space="preserve">${p_consent} = 'A.donne' </t>
-  </si>
-  <si>
     <t>${p_consent} = 'A.donne'  and ${p_collected_urine} = 'Oui'</t>
   </si>
   <si>
-    <t>${p_consent} = 'A.donne' and ${p_collected_urine} = 'Oui' and ${p_grading} != 'Negatif'</t>
-  </si>
-  <si>
     <t>${p_consent} = 'A.refuse'</t>
   </si>
   <si>
-    <t>${p_collected_stool} = 'Non' and ${p_collected_urine} = 'Non'</t>
-  </si>
-  <si>
     <t>calculate</t>
   </si>
   <si>
@@ -793,13 +763,25 @@
     <t>Cet identifiant est déjà utilisé</t>
   </si>
   <si>
-    <t>(2024 Octobre) - 2. SCH/STH – Enrôlement</t>
-  </si>
-  <si>
-    <t>bj_sch_sth_impact_2410_2_child</t>
-  </si>
-  <si>
-    <t>bj_p_2410</t>
+    <t>${p_collected_urine} = 'Non'</t>
+  </si>
+  <si>
+    <t>You have just entered a value that will cause the survey to end. Please collect the participant's urine samples.</t>
+  </si>
+  <si>
+    <t>Vous venez d'entrer une valeur qui entrainera la fin de l'enquête. Veuillez collecter les échantillons d'urine du participant.</t>
+  </si>
+  <si>
+    <t>bj_p_2410_021</t>
+  </si>
+  <si>
+    <t>bj_sch_sth_impact_2410_2_child_v21</t>
+  </si>
+  <si>
+    <t>(2024 Octobre) - 2. SCH/STH – Enrôlement V2.1</t>
+  </si>
+  <si>
+    <t>Les résultats Hemastix sont positives, l'urine doit être conservé.</t>
   </si>
 </sst>
 </file>
@@ -1354,13 +1336,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1410,7 @@
         <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1439,26 +1421,26 @@
         <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -1480,7 +1462,7 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="11" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="8"/>
@@ -1507,7 +1489,7 @@
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="8"/>
@@ -1521,7 +1503,7 @@
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="38" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1529,14 +1511,14 @@
         <v>17</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="8"/>
@@ -1550,7 +1532,7 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="38" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
@@ -1558,25 +1540,25 @@
         <v>17</v>
       </c>
       <c r="B6" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>177</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>183</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="35" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1585,7 +1567,7 @@
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="38" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1607,10 +1589,10 @@
     </row>
     <row r="8" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="10"/>
@@ -1622,7 +1604,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="M8" s="30"/>
       <c r="N8" s="9"/>
@@ -1630,17 +1612,17 @@
     </row>
     <row r="9" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="35" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
@@ -1655,10 +1637,10 @@
     </row>
     <row r="10" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="10"/>
@@ -1670,7 +1652,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="M10" s="30"/>
       <c r="N10" s="9"/>
@@ -1678,10 +1660,10 @@
     </row>
     <row r="11" spans="1:16" s="19" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="10"/>
@@ -1693,7 +1675,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="M11" s="30"/>
       <c r="N11" s="9"/>
@@ -1704,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>24</v>
@@ -1735,30 +1717,30 @@
         <v>30</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="35" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="37" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="30" t="s">
@@ -1769,17 +1751,17 @@
     </row>
     <row r="14" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="31" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="8"/>
@@ -1787,7 +1769,7 @@
       <c r="I14" s="10"/>
       <c r="J14" s="11"/>
       <c r="K14" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="30" t="s">
@@ -1801,7 +1783,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>35</v>
@@ -1816,7 +1798,7 @@
       <c r="I15" s="10"/>
       <c r="J15" s="11"/>
       <c r="K15" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="30" t="s">
@@ -1847,7 +1829,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>31</v>
@@ -1862,13 +1844,13 @@
         <v>33</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9" t="s">
@@ -1879,17 +1861,17 @@
     </row>
     <row r="18" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="31" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="8"/>
@@ -1897,7 +1879,7 @@
       <c r="I18" s="10"/>
       <c r="J18" s="11"/>
       <c r="K18" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="30" t="s">
@@ -1908,17 +1890,17 @@
     </row>
     <row r="19" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="31" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="8"/>
@@ -1926,7 +1908,7 @@
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
       <c r="K19" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -1938,31 +1920,31 @@
         <v>29</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="35" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="8"/>
       <c r="H20" s="19" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="K20" s="36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L20" s="36" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="M20" s="30" t="s">
         <v>16</v>
@@ -2007,31 +1989,27 @@
       <c r="N22" s="9"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="F23" s="11"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="26"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="37" t="s">
-        <v>223</v>
+      <c r="K23" s="36" t="s">
+        <v>215</v>
       </c>
       <c r="L23" s="8"/>
       <c r="M23" s="9" t="s">
@@ -2040,15 +2018,15 @@
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="11" t="s">
@@ -2060,88 +2038,84 @@
       <c r="I24" s="26"/>
       <c r="J24" s="27"/>
       <c r="K24" s="36" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="L24" s="8"/>
-      <c r="M24" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="M24" s="9"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>43</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="36" t="s">
-        <v>224</v>
-      </c>
+      <c r="H25" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="K25" s="36"/>
       <c r="L25" s="8"/>
       <c r="M25" s="9"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:16" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="36" t="s">
+    <row r="26" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="J26" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>49</v>
+        <v>233</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="25" t="s">
-        <v>50</v>
+        <v>234</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="12"/>
@@ -2149,35 +2123,33 @@
       <c r="I27" s="13"/>
       <c r="J27" s="14"/>
       <c r="K27" s="37" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
     </row>
-    <row r="28" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="13"/>
       <c r="J28" s="14"/>
-      <c r="K28" s="37" t="s">
-        <v>227</v>
-      </c>
+      <c r="K28" s="8"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
@@ -2185,18 +2157,12 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>220</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>53</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="23"/>
-      <c r="E29" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="E29" s="25"/>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
@@ -2210,10 +2176,14 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
+        <v>49</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="D30" s="23"/>
       <c r="E30" s="25"/>
       <c r="F30" s="14"/>
@@ -2228,14 +2198,14 @@
       <c r="O30" s="12"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>55</v>
+      <c r="A31" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="25"/>
@@ -2249,29 +2219,6 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2299,7 +2246,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -2311,16 +2258,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2335,30 +2282,30 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2369,520 +2316,520 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="C24" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C39" s="33" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D40" s="33" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D41" s="33" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D42" s="33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D43" s="33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="33" t="s">
-        <v>168</v>
-      </c>
       <c r="C44" s="33" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2897,7 +2844,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2908,24 +2855,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>